<commit_message>
Añadido template al reader, parser casi acabado
</commit_message>
<xml_diff>
--- a/input/ejemplo.xlsx
+++ b/input/ejemplo.xlsx
@@ -3,18 +3,14 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\NFM_9\Desktop\Nachin\GitProjects\citizensLoader_i1b\src\main\resources\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="11310" windowHeight="3600"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="0"/>
+  <oleSize ref="A1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>Javier</t>
   </si>
@@ -32,17 +28,52 @@
     <t>Muhlach</t>
   </si>
   <si>
-    <t>tira pedos</t>
+    <t>javier@email.com</t>
+  </si>
+  <si>
+    <t>española</t>
+  </si>
+  <si>
+    <t>71896514P</t>
+  </si>
+  <si>
+    <t>Pedro</t>
+  </si>
+  <si>
+    <t>Perez</t>
+  </si>
+  <si>
+    <t>pedro@email.com</t>
+  </si>
+  <si>
+    <t>07/01/1995</t>
+  </si>
+  <si>
+    <t>30/03/2004</t>
+  </si>
+  <si>
+    <t>rumana</t>
+  </si>
+  <si>
+    <t>61478945J</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -65,13 +96,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -350,26 +385,65 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2">
+        <v>5</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C1" r:id="rId1"/>
+    <hyperlink ref="C2" r:id="rId2"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Solving on log´s path exception and changing input to see if log is working
</commit_message>
<xml_diff>
--- a/input/ejemplo.xlsx
+++ b/input/ejemplo.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\NFM_9\Desktop\Nachin\GitProjects\citizensLoader_i1b\input\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\javie\Desktop\ASW\citizensLoader_i1b\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="14">
   <si>
     <t>Javier</t>
   </si>
@@ -71,7 +71,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -395,10 +395,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -459,10 +459,37 @@
         <v>5</v>
       </c>
     </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F3" t="s">
+        <v>3</v>
+      </c>
+      <c r="G3" t="s">
+        <v>12</v>
+      </c>
+      <c r="H3">
+        <v>24</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="D1" r:id="rId1"/>
     <hyperlink ref="D2" r:id="rId2"/>
+    <hyperlink ref="D3" r:id="rId3"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Algunos cambio en el log
</commit_message>
<xml_diff>
--- a/input/ejemplo.xlsx
+++ b/input/ejemplo.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\javie\Desktop\ASW\citizensLoader_i1b\input\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\NFM_9\Desktop\Nachin\GitProjects\citizensLoader_i1b\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="14">
   <si>
     <t>Javier</t>
   </si>
@@ -71,7 +71,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -398,13 +398,13 @@
   <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="H1" sqref="H1:H1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="4" max="4" width="20.7109375" customWidth="1"/>
-    <col min="7" max="7" width="18.42578125" customWidth="1"/>
+    <col min="6" max="6" width="18.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
@@ -424,9 +424,6 @@
         <v>4</v>
       </c>
       <c r="F1" t="s">
-        <v>3</v>
-      </c>
-      <c r="G1" t="s">
         <v>12</v>
       </c>
       <c r="H1">
@@ -450,10 +447,10 @@
         <v>11</v>
       </c>
       <c r="F2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G2" t="s">
         <v>10</v>
-      </c>
-      <c r="G2" t="s">
-        <v>13</v>
       </c>
       <c r="H2">
         <v>5</v>
@@ -476,10 +473,10 @@
         <v>4</v>
       </c>
       <c r="F3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G3" t="s">
         <v>3</v>
-      </c>
-      <c r="G3" t="s">
-        <v>12</v>
       </c>
       <c r="H3">
         <v>24</v>

</xml_diff>